<commit_message>
two ways to initialize_page_view
way 1:
rake db:initialize_page_view

way 2:
require "#{Rails.root}/lib/page_view.rb"
set_page_view
</commit_message>
<xml_diff>
--- a/lib/page_view.xlsx
+++ b/lib/page_view.xlsx
@@ -2589,8 +2589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>